<commit_message>
commit first iternation housing rent  _ 2011 03
</commit_message>
<xml_diff>
--- a/rent_library.xlsx
+++ b/rent_library.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_R\Real_estate\real_estate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22CD2F3-AB7F-490A-BB26-522C0D2EBC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4D0318-39D9-4689-A8FF-A8E9C4F9DD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{07813744-485E-40CA-9C87-172D5E7C2A54}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{07813744-485E-40CA-9C87-172D5E7C2A54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="directory" sheetId="2" r:id="rId2"/>
+    <sheet name="column_name_rename" sheetId="3" r:id="rId3"/>
+    <sheet name="rename_2011" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="128">
   <si>
     <t>Quarter</t>
   </si>
@@ -229,6 +231,198 @@
   </si>
   <si>
     <t>PC</t>
+  </si>
+  <si>
+    <t>col_names</t>
+  </si>
+  <si>
+    <t>metro/rest_of_state</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>1BR_flats_counts</t>
+  </si>
+  <si>
+    <t>2BR_flats_counts</t>
+  </si>
+  <si>
+    <t>2BR_flats_median</t>
+  </si>
+  <si>
+    <t>1BR_flats_median</t>
+  </si>
+  <si>
+    <t>3BR_flats_counts</t>
+  </si>
+  <si>
+    <t>3BR_flats_median</t>
+  </si>
+  <si>
+    <t>4BR_flats_counts</t>
+  </si>
+  <si>
+    <t>4BR_flats_median</t>
+  </si>
+  <si>
+    <t>flat_unknown_BR_counts</t>
+  </si>
+  <si>
+    <t>flat_unknow_BR_median</t>
+  </si>
+  <si>
+    <t>total_flats_counts</t>
+  </si>
+  <si>
+    <t>total_flats_median</t>
+  </si>
+  <si>
+    <t>1BR_houses_counts</t>
+  </si>
+  <si>
+    <t>1BR_houses_median</t>
+  </si>
+  <si>
+    <t>2BR_houses_counts</t>
+  </si>
+  <si>
+    <t>2BR_houses_median</t>
+  </si>
+  <si>
+    <t>3BR_houses_counts</t>
+  </si>
+  <si>
+    <t>3BR_houses_median</t>
+  </si>
+  <si>
+    <t>4BR_houses_counts</t>
+  </si>
+  <si>
+    <t>4BR_houses_median</t>
+  </si>
+  <si>
+    <t>house_unknown_BR_counts</t>
+  </si>
+  <si>
+    <t>house_unknow_BR_median</t>
+  </si>
+  <si>
+    <t>total_houses_counts</t>
+  </si>
+  <si>
+    <t>total_houses_median</t>
+  </si>
+  <si>
+    <t>Total_count</t>
+  </si>
+  <si>
+    <t>Total_unknown</t>
+  </si>
+  <si>
+    <t>quarter</t>
+  </si>
+  <si>
+    <t>metro_rest_of_state</t>
+  </si>
+  <si>
+    <t>Other_unknown_counts</t>
+  </si>
+  <si>
+    <t>Other_unknown_median</t>
+  </si>
+  <si>
+    <t>new_name</t>
+  </si>
+  <si>
+    <t>old_name</t>
+  </si>
+  <si>
+    <t>Metro/Rest of State</t>
+  </si>
+  <si>
+    <t>1 BR  Flats</t>
+  </si>
+  <si>
+    <t>...4</t>
+  </si>
+  <si>
+    <t>2 BR Flats</t>
+  </si>
+  <si>
+    <t>...6</t>
+  </si>
+  <si>
+    <t>3 BR Flats</t>
+  </si>
+  <si>
+    <t>...8</t>
+  </si>
+  <si>
+    <t>4+ BR Flats</t>
+  </si>
+  <si>
+    <t>...10</t>
+  </si>
+  <si>
+    <t>Flat unknown BR</t>
+  </si>
+  <si>
+    <t>...12</t>
+  </si>
+  <si>
+    <t>Total Flats</t>
+  </si>
+  <si>
+    <t>...14</t>
+  </si>
+  <si>
+    <t>1 BR Houses</t>
+  </si>
+  <si>
+    <t>...16</t>
+  </si>
+  <si>
+    <t>2 BR Houses</t>
+  </si>
+  <si>
+    <t>...18</t>
+  </si>
+  <si>
+    <t>3 BR Houses</t>
+  </si>
+  <si>
+    <t>...20</t>
+  </si>
+  <si>
+    <t>4+ BR Houses</t>
+  </si>
+  <si>
+    <t>...22</t>
+  </si>
+  <si>
+    <t>House unknown BR</t>
+  </si>
+  <si>
+    <t>...24</t>
+  </si>
+  <si>
+    <t>Total Houses</t>
+  </si>
+  <si>
+    <t>...26</t>
+  </si>
+  <si>
+    <t>Other/Unknown</t>
+  </si>
+  <si>
+    <t>...28</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>...30</t>
   </si>
 </sst>
 </file>
@@ -968,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA145643-D84D-4B99-B1DD-1074F9BE070D}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -980,9 +1174,10 @@
     <col min="2" max="2" width="53.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.36328125" customWidth="1"/>
     <col min="4" max="4" width="23.36328125" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -998,67 +1193,70 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3">
-        <v>41974</v>
+        <v>40513</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E2">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3">
-        <v>42064</v>
+        <v>40603</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E3">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3">
-        <v>42156</v>
+        <v>40695</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E4">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3">
-        <v>40513</v>
+        <v>40787</v>
       </c>
       <c r="D5" t="s">
         <v>62</v>
@@ -1067,15 +1265,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3">
-        <v>40603</v>
+        <v>40878</v>
       </c>
       <c r="D6" t="s">
         <v>62</v>
@@ -1084,15 +1282,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3">
-        <v>40695</v>
+        <v>40969</v>
       </c>
       <c r="D7" t="s">
         <v>62</v>
@@ -1101,15 +1299,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3">
-        <v>40787</v>
+        <v>41061</v>
       </c>
       <c r="D8" t="s">
         <v>62</v>
@@ -1118,15 +1316,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3">
-        <v>40878</v>
+        <v>41153</v>
       </c>
       <c r="D9" t="s">
         <v>62</v>
@@ -1135,15 +1333,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3">
-        <v>40969</v>
+        <v>41244</v>
       </c>
       <c r="D10" t="s">
         <v>62</v>
@@ -1152,66 +1350,66 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3">
-        <v>41061</v>
+        <v>41334</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E11">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3">
-        <v>43709</v>
+        <v>41426</v>
       </c>
       <c r="D12" t="s">
         <v>61</v>
       </c>
       <c r="E12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3">
-        <v>43800</v>
+        <v>41518</v>
       </c>
       <c r="D13" t="s">
         <v>61</v>
       </c>
       <c r="E13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C14" s="3">
-        <v>42248</v>
+        <v>41609</v>
       </c>
       <c r="D14" t="s">
         <v>61</v>
@@ -1220,15 +1418,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3">
-        <v>42339</v>
+        <v>41699</v>
       </c>
       <c r="D15" t="s">
         <v>61</v>
@@ -1237,15 +1435,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3">
-        <v>42430</v>
+        <v>41791</v>
       </c>
       <c r="D16" t="s">
         <v>61</v>
@@ -1259,10 +1457,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3">
-        <v>42522</v>
+        <v>41883</v>
       </c>
       <c r="D17" t="s">
         <v>61</v>
@@ -1276,10 +1474,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C18" s="3">
-        <v>42614</v>
+        <v>41974</v>
       </c>
       <c r="D18" t="s">
         <v>61</v>
@@ -1293,10 +1491,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C19" s="3">
-        <v>42705</v>
+        <v>42064</v>
       </c>
       <c r="D19" t="s">
         <v>61</v>
@@ -1310,10 +1508,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C20" s="3">
-        <v>42795</v>
+        <v>42156</v>
       </c>
       <c r="D20" t="s">
         <v>61</v>
@@ -1327,10 +1525,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C21" s="3">
-        <v>42979</v>
+        <v>42248</v>
       </c>
       <c r="D21" t="s">
         <v>61</v>
@@ -1344,10 +1542,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C22" s="3">
-        <v>43070</v>
+        <v>42339</v>
       </c>
       <c r="D22" t="s">
         <v>61</v>
@@ -1361,10 +1559,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C23" s="3">
-        <v>43160</v>
+        <v>42430</v>
       </c>
       <c r="D23" t="s">
         <v>61</v>
@@ -1378,10 +1576,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C24" s="3">
-        <v>43344</v>
+        <v>42522</v>
       </c>
       <c r="D24" t="s">
         <v>61</v>
@@ -1395,10 +1593,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C25" s="3">
-        <v>43435</v>
+        <v>42614</v>
       </c>
       <c r="D25" t="s">
         <v>61</v>
@@ -1412,10 +1610,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C26" s="3">
-        <v>43525</v>
+        <v>42705</v>
       </c>
       <c r="D26" t="s">
         <v>61</v>
@@ -1429,10 +1627,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C27" s="3">
-        <v>43617</v>
+        <v>42795</v>
       </c>
       <c r="D27" t="s">
         <v>61</v>
@@ -1446,13 +1644,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C28" s="3">
-        <v>41153</v>
+        <v>42887</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E28">
         <v>19</v>
@@ -1463,13 +1661,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C29" s="3">
-        <v>41244</v>
+        <v>42979</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E29">
         <v>19</v>
@@ -1480,13 +1678,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C30" s="3">
-        <v>41334</v>
+        <v>43070</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E30">
         <v>19</v>
@@ -1497,10 +1695,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C31" s="3">
-        <v>41426</v>
+        <v>43160</v>
       </c>
       <c r="D31" t="s">
         <v>61</v>
@@ -1514,10 +1712,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C32" s="3">
-        <v>41518</v>
+        <v>43344</v>
       </c>
       <c r="D32" t="s">
         <v>61</v>
@@ -1531,10 +1729,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C33" s="3">
-        <v>41609</v>
+        <v>43435</v>
       </c>
       <c r="D33" t="s">
         <v>61</v>
@@ -1548,10 +1746,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C34" s="3">
-        <v>41699</v>
+        <v>43525</v>
       </c>
       <c r="D34" t="s">
         <v>61</v>
@@ -1565,10 +1763,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C35" s="3">
-        <v>41791</v>
+        <v>43617</v>
       </c>
       <c r="D35" t="s">
         <v>61</v>
@@ -1582,16 +1780,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C36" s="3">
-        <v>41883</v>
+        <v>43709</v>
       </c>
       <c r="D36" t="s">
         <v>61</v>
       </c>
       <c r="E36">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1599,10 +1797,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C37" s="3">
-        <v>43891</v>
+        <v>43800</v>
       </c>
       <c r="D37" t="s">
         <v>61</v>
@@ -1616,10 +1814,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38" s="3">
-        <v>43983</v>
+        <v>43891</v>
       </c>
       <c r="D38" t="s">
         <v>61</v>
@@ -1633,10 +1831,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" s="3">
-        <v>44075</v>
+        <v>43983</v>
       </c>
       <c r="D39" t="s">
         <v>61</v>
@@ -1650,13 +1848,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40" s="3">
-        <v>44166</v>
+        <v>44075</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E40">
         <v>12</v>
@@ -1667,10 +1865,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" s="3">
-        <v>44256</v>
+        <v>44166</v>
       </c>
       <c r="D41" t="s">
         <v>63</v>
@@ -1684,10 +1882,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C42" s="3">
-        <v>44348</v>
+        <v>44256</v>
       </c>
       <c r="D42" t="s">
         <v>63</v>
@@ -1701,10 +1899,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" s="3">
-        <v>44440</v>
+        <v>44348</v>
       </c>
       <c r="D43" t="s">
         <v>63</v>
@@ -1718,10 +1916,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" s="3">
-        <v>44531</v>
+        <v>44440</v>
       </c>
       <c r="D44" t="s">
         <v>63</v>
@@ -1735,10 +1933,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" s="3">
-        <v>44621</v>
+        <v>44531</v>
       </c>
       <c r="D45" t="s">
         <v>63</v>
@@ -1752,10 +1950,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C46" s="3">
-        <v>44713</v>
+        <v>44621</v>
       </c>
       <c r="D46" t="s">
         <v>63</v>
@@ -1769,10 +1967,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" s="3">
-        <v>44805</v>
+        <v>44713</v>
       </c>
       <c r="D47" t="s">
         <v>63</v>
@@ -1786,10 +1984,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48" s="3">
-        <v>44896</v>
+        <v>44805</v>
       </c>
       <c r="D48" t="s">
         <v>63</v>
@@ -1803,10 +2001,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" s="3">
-        <v>44986</v>
+        <v>44896</v>
       </c>
       <c r="D49" t="s">
         <v>63</v>
@@ -1820,10 +2018,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C50" s="3">
-        <v>45078</v>
+        <v>44986</v>
       </c>
       <c r="D50" t="s">
         <v>63</v>
@@ -1837,10 +2035,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C51" s="3">
-        <v>45170</v>
+        <v>45078</v>
       </c>
       <c r="D51" t="s">
         <v>63</v>
@@ -1854,10 +2052,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52" s="3">
-        <v>45261</v>
+        <v>45170</v>
       </c>
       <c r="D52" t="s">
         <v>63</v>
@@ -1871,10 +2069,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C53" s="3">
-        <v>45352</v>
+        <v>45261</v>
       </c>
       <c r="D53" t="s">
         <v>63</v>
@@ -1888,10 +2086,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C54" s="3">
-        <v>45444</v>
+        <v>45352</v>
       </c>
       <c r="D54" t="s">
         <v>63</v>
@@ -1905,22 +2103,350 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C55" s="3">
-        <v>42887</v>
+        <v>45444</v>
       </c>
       <c r="D55" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E55">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B55">
-    <sortCondition ref="B2:B55"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E55">
+    <sortCondition ref="C2:C55"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B2B4F8-84A7-42A5-AD2F-D10CF868A00A}">
+  <dimension ref="B1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B1" s="3">
+        <v>40513</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65798D6-DDCA-4973-BAFA-2D28352840F3}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J32" sqref="H32:J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commit rent library fix
</commit_message>
<xml_diff>
--- a/rent_library.xlsx
+++ b/rent_library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_R\Real_estate\real_estate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4140CEE0-656E-44D9-B287-9C4E7294F3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8E1CB4-688D-4E37-B625-252A4321BADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="4130" windowWidth="28710" windowHeight="15350" activeTab="2" xr2:uid="{07813744-485E-40CA-9C87-172D5E7C2A54}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{07813744-485E-40CA-9C87-172D5E7C2A54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="129">
   <si>
     <t>Quarter</t>
   </si>
@@ -436,10 +436,16 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1168,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA145643-D84D-4B99-B1DD-1074F9BE070D}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:F8"/>
+    <sheetView topLeftCell="A17" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1178,7 +1184,7 @@
     <col min="2" max="2" width="53.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.36328125" customWidth="1"/>
     <col min="4" max="4" width="23.36328125" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" customWidth="1"/>
+    <col min="6" max="6" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -1357,6 +1363,9 @@
       <c r="E9">
         <v>19</v>
       </c>
+      <c r="F9" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1374,6 +1383,9 @@
       <c r="E10">
         <v>19</v>
       </c>
+      <c r="F10" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -1391,6 +1403,9 @@
       <c r="E11">
         <v>19</v>
       </c>
+      <c r="F11" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -1408,6 +1423,9 @@
       <c r="E12">
         <v>19</v>
       </c>
+      <c r="F12" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -1425,6 +1443,9 @@
       <c r="E13">
         <v>19</v>
       </c>
+      <c r="F13" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -1442,6 +1463,9 @@
       <c r="E14">
         <v>19</v>
       </c>
+      <c r="F14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -1459,6 +1483,9 @@
       <c r="E15">
         <v>19</v>
       </c>
+      <c r="F15" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -1476,8 +1503,11 @@
       <c r="E16">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1493,8 +1523,11 @@
       <c r="E17">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1510,8 +1543,11 @@
       <c r="E18">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1527,8 +1563,11 @@
       <c r="E19">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1544,8 +1583,11 @@
       <c r="E20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1561,8 +1603,11 @@
       <c r="E21">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1578,8 +1623,11 @@
       <c r="E22">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1595,8 +1643,11 @@
       <c r="E23">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1612,8 +1663,11 @@
       <c r="E24">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1629,8 +1683,11 @@
       <c r="E25">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1646,8 +1703,11 @@
       <c r="E26">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1663,8 +1723,11 @@
       <c r="E27">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1680,8 +1743,11 @@
       <c r="E28">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1697,8 +1763,11 @@
       <c r="E29">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1714,8 +1783,11 @@
       <c r="E30">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1731,8 +1803,11 @@
       <c r="E31">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1748,8 +1823,11 @@
       <c r="E32">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1765,8 +1843,11 @@
       <c r="E33">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1782,8 +1863,11 @@
       <c r="E34">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1799,8 +1883,11 @@
       <c r="E35">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1816,8 +1903,11 @@
       <c r="E36">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1833,8 +1923,11 @@
       <c r="E37">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1850,8 +1943,11 @@
       <c r="E38">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1867,8 +1963,11 @@
       <c r="E39">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1884,8 +1983,11 @@
       <c r="E40">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F40" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1902,7 +2004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1919,7 +2021,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1936,7 +2038,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1953,7 +2055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1970,7 +2072,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1987,7 +2089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2004,7 +2106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2144,19 +2246,24 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E55">
     <sortCondition ref="C2:C55"/>
   </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7862416-338A-4A69-9E9D-52FEB2010937}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F8"/>
+      <selection activeCell="A41" sqref="A41:A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="54.90625" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2315,6 +2422,646 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3">
+        <v>41153</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="3">
+        <v>41244</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3">
+        <v>41334</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3">
+        <v>41426</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3">
+        <v>41518</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="3">
+        <v>41609</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3">
+        <v>41699</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="3">
+        <v>41791</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="3">
+        <v>41883</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3">
+        <v>41974</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3">
+        <v>42064</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3">
+        <v>42156</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="3">
+        <v>42248</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="3">
+        <v>42339</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="3">
+        <v>42430</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="3">
+        <v>42522</v>
+      </c>
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24">
+        <v>19</v>
+      </c>
+      <c r="F24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="3">
+        <v>42614</v>
+      </c>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="3">
+        <v>42705</v>
+      </c>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26">
+        <v>19</v>
+      </c>
+      <c r="F26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="3">
+        <v>42795</v>
+      </c>
+      <c r="D27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="3">
+        <v>42887</v>
+      </c>
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28">
+        <v>19</v>
+      </c>
+      <c r="F28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="3">
+        <v>42979</v>
+      </c>
+      <c r="D29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29">
+        <v>19</v>
+      </c>
+      <c r="F29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="3">
+        <v>43070</v>
+      </c>
+      <c r="D30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30">
+        <v>19</v>
+      </c>
+      <c r="F30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="3">
+        <v>43160</v>
+      </c>
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31">
+        <v>19</v>
+      </c>
+      <c r="F31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="3">
+        <v>43344</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="3">
+        <v>43435</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="3">
+        <v>43525</v>
+      </c>
+      <c r="D34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34">
+        <v>19</v>
+      </c>
+      <c r="F34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="3">
+        <v>43617</v>
+      </c>
+      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35">
+        <v>19</v>
+      </c>
+      <c r="F35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="3">
+        <v>43709</v>
+      </c>
+      <c r="D36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="3">
+        <v>43800</v>
+      </c>
+      <c r="D37" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37">
+        <v>12</v>
+      </c>
+      <c r="F37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="3">
+        <v>43891</v>
+      </c>
+      <c r="D38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="3">
+        <v>43983</v>
+      </c>
+      <c r="D39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="3">
+        <v>44075</v>
+      </c>
+      <c r="D40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40">
+        <v>12</v>
+      </c>
+      <c r="F40" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2381,7 +3128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65798D6-DDCA-4973-BAFA-2D28352840F3}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ingestion 2024 style fix column name but igore metro or rest of state
</commit_message>
<xml_diff>
--- a/rent_library.xlsx
+++ b/rent_library.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_R\Real_estate\real_estate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8E1CB4-688D-4E37-B625-252A4321BADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18661B9-7FE5-497A-A696-EB84B8C9FE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{07813744-485E-40CA-9C87-172D5E7C2A54}"/>
+    <workbookView xWindow="19010" yWindow="0" windowWidth="19380" windowHeight="20970" firstSheet="3" activeTab="6" xr2:uid="{07813744-485E-40CA-9C87-172D5E7C2A54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="directory" sheetId="2" r:id="rId2"/>
     <sheet name="directory_try" sheetId="5" r:id="rId3"/>
-    <sheet name="column_name_rename" sheetId="3" r:id="rId4"/>
-    <sheet name="rename_2011" sheetId="4" r:id="rId5"/>
+    <sheet name="directory_2024" sheetId="7" r:id="rId4"/>
+    <sheet name="column_name_rename" sheetId="3" r:id="rId5"/>
+    <sheet name="rename_2011" sheetId="4" r:id="rId6"/>
+    <sheet name="rename_2024" sheetId="6" r:id="rId7"/>
+    <sheet name="metroX" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="155">
   <si>
     <t>Quarter</t>
   </si>
@@ -427,16 +430,95 @@
   </si>
   <si>
     <t>rename_2011</t>
+  </si>
+  <si>
+    <t>rename_2024</t>
+  </si>
+  <si>
+    <t>...3</t>
+  </si>
+  <si>
+    <t>...5</t>
+  </si>
+  <si>
+    <t>...7</t>
+  </si>
+  <si>
+    <t>...9</t>
+  </si>
+  <si>
+    <t>...11</t>
+  </si>
+  <si>
+    <t>...15</t>
+  </si>
+  <si>
+    <t>...17</t>
+  </si>
+  <si>
+    <t>...19</t>
+  </si>
+  <si>
+    <t>...21</t>
+  </si>
+  <si>
+    <t>...23</t>
+  </si>
+  <si>
+    <t>...27</t>
+  </si>
+  <si>
+    <t>...2</t>
+  </si>
+  <si>
+    <t>...13</t>
+  </si>
+  <si>
+    <t>...25</t>
+  </si>
+  <si>
+    <t>...29</t>
+  </si>
+  <si>
+    <t>...31</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Country Total</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Rest_of_state</t>
+  </si>
+  <si>
+    <t>Metro Total</t>
+  </si>
+  <si>
+    <t>Delete1</t>
+  </si>
+  <si>
+    <t>Delete2</t>
+  </si>
+  <si>
+    <t>Total_Count</t>
+  </si>
+  <si>
+    <t>Total_Median</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="170" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,6 +531,16 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -468,8 +560,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -477,8 +573,12 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Currency 2" xfId="4" xr:uid="{14BB1EFC-9084-481D-AD08-89D09998AE7E}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{6D323169-57AF-4DA7-8E2D-192BAD1BCD58}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{B9039A80-9607-45A2-84AB-CBA13B9103B3}"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{665B0A30-5980-4E76-BC0C-630C67BCC50E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1174,8 +1274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA145643-D84D-4B99-B1DD-1074F9BE070D}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A55"/>
+    <sheetView topLeftCell="B28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2253,10 +2353,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7862416-338A-4A69-9E9D-52FEB2010937}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:A55"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3065,12 +3165,424 @@
         <v>128</v>
       </c>
     </row>
+    <row r="58" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C773356D-0F65-45D6-94FD-903551291D21}">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="54.90625" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44166</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3">
+        <v>44256</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44348</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44440</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44531</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="3">
+        <v>44621</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44713</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44805</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3">
+        <v>44896</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3">
+        <v>44986</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45078</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45170</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45261</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45352</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45444</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C40" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B2B4F8-84A7-42A5-AD2F-D10CF868A00A}">
   <dimension ref="B1:B7"/>
   <sheetViews>
@@ -3124,12 +3636,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65798D6-DDCA-4973-BAFA-2D28352840F3}">
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B30" sqref="B30:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3396,4 +3908,2347 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9392492D-C307-4343-BED9-8FAD1A381722}">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9415D53-1FA2-499A-BD09-F544ECCD8C23}">
+  <dimension ref="A1:F255"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>5000</v>
+      </c>
+      <c r="B2">
+        <v>5118</v>
+      </c>
+      <c r="F2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>5006</v>
+      </c>
+      <c r="B3">
+        <v>5133</v>
+      </c>
+      <c r="F3">
+        <v>5006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5007</v>
+      </c>
+      <c r="B4">
+        <v>5153</v>
+      </c>
+      <c r="F4">
+        <v>5007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>5008</v>
+      </c>
+      <c r="B5">
+        <v>5157</v>
+      </c>
+      <c r="F5">
+        <v>5008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5009</v>
+      </c>
+      <c r="B6">
+        <v>5172</v>
+      </c>
+      <c r="F6">
+        <v>5009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5010</v>
+      </c>
+      <c r="B7">
+        <v>5201</v>
+      </c>
+      <c r="F7">
+        <v>5010</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>5011</v>
+      </c>
+      <c r="B8">
+        <v>5202</v>
+      </c>
+      <c r="F8">
+        <v>5011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>5012</v>
+      </c>
+      <c r="B9">
+        <v>5203</v>
+      </c>
+      <c r="F9">
+        <v>5012</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>5013</v>
+      </c>
+      <c r="B10">
+        <v>5204</v>
+      </c>
+      <c r="F10">
+        <v>5013</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>5014</v>
+      </c>
+      <c r="B11">
+        <v>5210</v>
+      </c>
+      <c r="F11">
+        <v>5014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>5015</v>
+      </c>
+      <c r="B12">
+        <v>5211</v>
+      </c>
+      <c r="F12">
+        <v>5015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>5016</v>
+      </c>
+      <c r="B13">
+        <v>5212</v>
+      </c>
+      <c r="F13">
+        <v>5016</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>5017</v>
+      </c>
+      <c r="B14">
+        <v>5213</v>
+      </c>
+      <c r="F14">
+        <v>5017</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>5018</v>
+      </c>
+      <c r="B15">
+        <v>5214</v>
+      </c>
+      <c r="F15">
+        <v>5018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>5019</v>
+      </c>
+      <c r="B16">
+        <v>5220</v>
+      </c>
+      <c r="F16">
+        <v>5019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>5020</v>
+      </c>
+      <c r="B17">
+        <v>5221</v>
+      </c>
+      <c r="F17">
+        <v>5020</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>5021</v>
+      </c>
+      <c r="B18">
+        <v>5222</v>
+      </c>
+      <c r="F18">
+        <v>5021</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>5022</v>
+      </c>
+      <c r="B19">
+        <v>5223</v>
+      </c>
+      <c r="F19">
+        <v>5022</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>5023</v>
+      </c>
+      <c r="B20">
+        <v>5233</v>
+      </c>
+      <c r="F20">
+        <v>5023</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>5024</v>
+      </c>
+      <c r="B21">
+        <v>5234</v>
+      </c>
+      <c r="F21">
+        <v>5024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>5025</v>
+      </c>
+      <c r="B22">
+        <v>5235</v>
+      </c>
+      <c r="F22">
+        <v>5025</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>5031</v>
+      </c>
+      <c r="B23">
+        <v>5236</v>
+      </c>
+      <c r="F23">
+        <v>5031</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>5032</v>
+      </c>
+      <c r="B24">
+        <v>5238</v>
+      </c>
+      <c r="F24">
+        <v>5032</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>5033</v>
+      </c>
+      <c r="B25">
+        <v>5240</v>
+      </c>
+      <c r="F25">
+        <v>5033</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>5034</v>
+      </c>
+      <c r="B26">
+        <v>5241</v>
+      </c>
+      <c r="F26">
+        <v>5034</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>5035</v>
+      </c>
+      <c r="B27">
+        <v>5242</v>
+      </c>
+      <c r="F27">
+        <v>5035</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>5037</v>
+      </c>
+      <c r="B28">
+        <v>5243</v>
+      </c>
+      <c r="F28">
+        <v>5037</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>5038</v>
+      </c>
+      <c r="B29">
+        <v>5244</v>
+      </c>
+      <c r="F29">
+        <v>5038</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>5039</v>
+      </c>
+      <c r="B30">
+        <v>5245</v>
+      </c>
+      <c r="F30">
+        <v>5039</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>5040</v>
+      </c>
+      <c r="B31">
+        <v>5250</v>
+      </c>
+      <c r="F31">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>5041</v>
+      </c>
+      <c r="B32">
+        <v>5251</v>
+      </c>
+      <c r="F32">
+        <v>5041</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>5042</v>
+      </c>
+      <c r="B33">
+        <v>5252</v>
+      </c>
+      <c r="F33">
+        <v>5042</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>5043</v>
+      </c>
+      <c r="B34">
+        <v>5253</v>
+      </c>
+      <c r="F34">
+        <v>5043</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>5044</v>
+      </c>
+      <c r="B35">
+        <v>5254</v>
+      </c>
+      <c r="F35">
+        <v>5044</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>5045</v>
+      </c>
+      <c r="B36">
+        <v>5255</v>
+      </c>
+      <c r="F36">
+        <v>5045</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>5046</v>
+      </c>
+      <c r="B37">
+        <v>5256</v>
+      </c>
+      <c r="F37">
+        <v>5046</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>5047</v>
+      </c>
+      <c r="B38">
+        <v>5259</v>
+      </c>
+      <c r="F38">
+        <v>5047</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>5048</v>
+      </c>
+      <c r="B39">
+        <v>5260</v>
+      </c>
+      <c r="F39">
+        <v>5048</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>5049</v>
+      </c>
+      <c r="B40">
+        <v>5261</v>
+      </c>
+      <c r="F40">
+        <v>5049</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>5050</v>
+      </c>
+      <c r="B41">
+        <v>5263</v>
+      </c>
+      <c r="F41">
+        <v>5050</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>5051</v>
+      </c>
+      <c r="B42">
+        <v>5264</v>
+      </c>
+      <c r="F42">
+        <v>5051</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>5052</v>
+      </c>
+      <c r="B43">
+        <v>5265</v>
+      </c>
+      <c r="F43">
+        <v>5052</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>5061</v>
+      </c>
+      <c r="B44">
+        <v>5266</v>
+      </c>
+      <c r="F44">
+        <v>5061</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>5062</v>
+      </c>
+      <c r="B45">
+        <v>5267</v>
+      </c>
+      <c r="F45">
+        <v>5062</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>5063</v>
+      </c>
+      <c r="B46">
+        <v>5268</v>
+      </c>
+      <c r="F46">
+        <v>5063</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>5064</v>
+      </c>
+      <c r="B47">
+        <v>5271</v>
+      </c>
+      <c r="F47">
+        <v>5064</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>5065</v>
+      </c>
+      <c r="B48">
+        <v>5275</v>
+      </c>
+      <c r="F48">
+        <v>5065</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>5066</v>
+      </c>
+      <c r="B49">
+        <v>5276</v>
+      </c>
+      <c r="F49">
+        <v>5066</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>5067</v>
+      </c>
+      <c r="B50">
+        <v>5277</v>
+      </c>
+      <c r="F50">
+        <v>5067</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>5068</v>
+      </c>
+      <c r="B51">
+        <v>5278</v>
+      </c>
+      <c r="F51">
+        <v>5068</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>5069</v>
+      </c>
+      <c r="B52">
+        <v>5279</v>
+      </c>
+      <c r="F52">
+        <v>5069</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>5070</v>
+      </c>
+      <c r="B53">
+        <v>5280</v>
+      </c>
+      <c r="F53">
+        <v>5070</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>5072</v>
+      </c>
+      <c r="B54">
+        <v>5290</v>
+      </c>
+      <c r="F54">
+        <v>5072</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>5073</v>
+      </c>
+      <c r="B55">
+        <v>5291</v>
+      </c>
+      <c r="F55">
+        <v>5073</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>5074</v>
+      </c>
+      <c r="B56">
+        <v>5302</v>
+      </c>
+      <c r="F56">
+        <v>5074</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>5075</v>
+      </c>
+      <c r="B57">
+        <v>5304</v>
+      </c>
+      <c r="F57">
+        <v>5075</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>5076</v>
+      </c>
+      <c r="B58">
+        <v>5311</v>
+      </c>
+      <c r="F58">
+        <v>5076</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>5081</v>
+      </c>
+      <c r="B59">
+        <v>5320</v>
+      </c>
+      <c r="F59">
+        <v>5081</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>5082</v>
+      </c>
+      <c r="B60">
+        <v>5321</v>
+      </c>
+      <c r="F60">
+        <v>5082</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>5083</v>
+      </c>
+      <c r="B61">
+        <v>5330</v>
+      </c>
+      <c r="F61">
+        <v>5083</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>5084</v>
+      </c>
+      <c r="B62">
+        <v>5333</v>
+      </c>
+      <c r="F62">
+        <v>5084</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>5085</v>
+      </c>
+      <c r="B63">
+        <v>5340</v>
+      </c>
+      <c r="F63">
+        <v>5085</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>5086</v>
+      </c>
+      <c r="B64">
+        <v>5341</v>
+      </c>
+      <c r="F64">
+        <v>5086</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>5087</v>
+      </c>
+      <c r="B65">
+        <v>5342</v>
+      </c>
+      <c r="F65">
+        <v>5087</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>5088</v>
+      </c>
+      <c r="B66">
+        <v>5343</v>
+      </c>
+      <c r="F66">
+        <v>5088</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>5089</v>
+      </c>
+      <c r="B67">
+        <v>5344</v>
+      </c>
+      <c r="F67">
+        <v>5089</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>5090</v>
+      </c>
+      <c r="B68">
+        <v>5345</v>
+      </c>
+      <c r="F68">
+        <v>5090</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>5091</v>
+      </c>
+      <c r="B69">
+        <v>5350</v>
+      </c>
+      <c r="F69">
+        <v>5091</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>5092</v>
+      </c>
+      <c r="B70">
+        <v>5351</v>
+      </c>
+      <c r="F70">
+        <v>5092</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>5093</v>
+      </c>
+      <c r="B71">
+        <v>5352</v>
+      </c>
+      <c r="F71">
+        <v>5093</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>5094</v>
+      </c>
+      <c r="B72">
+        <v>5353</v>
+      </c>
+      <c r="F72">
+        <v>5094</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>5095</v>
+      </c>
+      <c r="B73">
+        <v>5355</v>
+      </c>
+      <c r="F73">
+        <v>5095</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>5096</v>
+      </c>
+      <c r="B74">
+        <v>5356</v>
+      </c>
+      <c r="F74">
+        <v>5096</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>5097</v>
+      </c>
+      <c r="B75">
+        <v>5360</v>
+      </c>
+      <c r="F75">
+        <v>5097</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>5098</v>
+      </c>
+      <c r="B76">
+        <v>5371</v>
+      </c>
+      <c r="F76">
+        <v>5098</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>5107</v>
+      </c>
+      <c r="B77">
+        <v>5372</v>
+      </c>
+      <c r="F77">
+        <v>5107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>5108</v>
+      </c>
+      <c r="B78">
+        <v>5373</v>
+      </c>
+      <c r="F78">
+        <v>5108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>5109</v>
+      </c>
+      <c r="B79">
+        <v>5374</v>
+      </c>
+      <c r="F79">
+        <v>5109</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>5110</v>
+      </c>
+      <c r="B80">
+        <v>5400</v>
+      </c>
+      <c r="F80">
+        <v>5110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>5112</v>
+      </c>
+      <c r="B81">
+        <v>5401</v>
+      </c>
+      <c r="F81">
+        <v>5112</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>5113</v>
+      </c>
+      <c r="B82">
+        <v>5412</v>
+      </c>
+      <c r="F82">
+        <v>5113</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>5114</v>
+      </c>
+      <c r="B83">
+        <v>5413</v>
+      </c>
+      <c r="F83">
+        <v>5114</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>5115</v>
+      </c>
+      <c r="B84">
+        <v>5417</v>
+      </c>
+      <c r="F84">
+        <v>5115</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>5116</v>
+      </c>
+      <c r="B85">
+        <v>5419</v>
+      </c>
+      <c r="F85">
+        <v>5116</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>5117</v>
+      </c>
+      <c r="B86">
+        <v>5422</v>
+      </c>
+      <c r="F86">
+        <v>5117</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>5118</v>
+      </c>
+      <c r="B87">
+        <v>5431</v>
+      </c>
+      <c r="F87">
+        <v>5118</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>5120</v>
+      </c>
+      <c r="B88">
+        <v>5433</v>
+      </c>
+      <c r="F88">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>5121</v>
+      </c>
+      <c r="B89">
+        <v>5451</v>
+      </c>
+      <c r="F89">
+        <v>5121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>5125</v>
+      </c>
+      <c r="B90">
+        <v>5452</v>
+      </c>
+      <c r="F90">
+        <v>5125</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>5126</v>
+      </c>
+      <c r="B91">
+        <v>5453</v>
+      </c>
+      <c r="F91">
+        <v>5126</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>5127</v>
+      </c>
+      <c r="B92">
+        <v>5460</v>
+      </c>
+      <c r="F92">
+        <v>5127</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>5138</v>
+      </c>
+      <c r="B93">
+        <v>5461</v>
+      </c>
+      <c r="F93">
+        <v>5141</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>5140</v>
+      </c>
+      <c r="B94">
+        <v>5462</v>
+      </c>
+      <c r="F94">
+        <v>5142</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>5142</v>
+      </c>
+      <c r="B95">
+        <v>5464</v>
+      </c>
+      <c r="F95">
+        <v>5144</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>5150</v>
+      </c>
+      <c r="B96">
+        <v>5473</v>
+      </c>
+      <c r="F96">
+        <v>5150</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>5152</v>
+      </c>
+      <c r="B97">
+        <v>5480</v>
+      </c>
+      <c r="F97">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>5153</v>
+      </c>
+      <c r="B98">
+        <v>5481</v>
+      </c>
+      <c r="F98">
+        <v>5152</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>5154</v>
+      </c>
+      <c r="B99">
+        <v>5483</v>
+      </c>
+      <c r="F99">
+        <v>5153</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>5155</v>
+      </c>
+      <c r="B100">
+        <v>5491</v>
+      </c>
+      <c r="F100">
+        <v>5154</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>5157</v>
+      </c>
+      <c r="B101">
+        <v>5495</v>
+      </c>
+      <c r="F101">
+        <v>5155</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>5158</v>
+      </c>
+      <c r="B102">
+        <v>5501</v>
+      </c>
+      <c r="F102">
+        <v>5157</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>5159</v>
+      </c>
+      <c r="B103">
+        <v>5502</v>
+      </c>
+      <c r="F103">
+        <v>5158</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>5161</v>
+      </c>
+      <c r="B104">
+        <v>5522</v>
+      </c>
+      <c r="F104">
+        <v>5159</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>5162</v>
+      </c>
+      <c r="B105">
+        <v>5523</v>
+      </c>
+      <c r="F105">
+        <v>5161</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>5163</v>
+      </c>
+      <c r="B106">
+        <v>5540</v>
+      </c>
+      <c r="F106">
+        <v>5162</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>5164</v>
+      </c>
+      <c r="B107">
+        <v>5550</v>
+      </c>
+      <c r="F107">
+        <v>5163</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>5165</v>
+      </c>
+      <c r="B108">
+        <v>5554</v>
+      </c>
+      <c r="F108">
+        <v>5164</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>5166</v>
+      </c>
+      <c r="B109">
+        <v>5556</v>
+      </c>
+      <c r="F109">
+        <v>5165</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>5167</v>
+      </c>
+      <c r="B110">
+        <v>5558</v>
+      </c>
+      <c r="F110">
+        <v>5166</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>5168</v>
+      </c>
+      <c r="B111">
+        <v>5570</v>
+      </c>
+      <c r="F111">
+        <v>5167</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>5169</v>
+      </c>
+      <c r="B112">
+        <v>5571</v>
+      </c>
+      <c r="F112">
+        <v>5168</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>5170</v>
+      </c>
+      <c r="B113">
+        <v>5573</v>
+      </c>
+      <c r="F113">
+        <v>5169</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>5171</v>
+      </c>
+      <c r="B114">
+        <v>5575</v>
+      </c>
+      <c r="F114">
+        <v>5170</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>5172</v>
+      </c>
+      <c r="B115">
+        <v>5576</v>
+      </c>
+      <c r="F115">
+        <v>5171</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>5173</v>
+      </c>
+      <c r="B116">
+        <v>5580</v>
+      </c>
+      <c r="F116">
+        <v>5172</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>5174</v>
+      </c>
+      <c r="B117">
+        <v>5581</v>
+      </c>
+      <c r="F117">
+        <v>5173</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B118">
+        <v>5583</v>
+      </c>
+      <c r="F118">
+        <v>5174</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B119">
+        <v>5600</v>
+      </c>
+      <c r="F119" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B120">
+        <v>5602</v>
+      </c>
+      <c r="F120" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B121">
+        <v>5603</v>
+      </c>
+      <c r="F121">
+        <v>5118</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B122">
+        <v>5605</v>
+      </c>
+      <c r="F122">
+        <v>5133</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B123">
+        <v>5606</v>
+      </c>
+      <c r="F123">
+        <v>5153</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B124">
+        <v>5607</v>
+      </c>
+      <c r="F124">
+        <v>5172</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B125">
+        <v>5608</v>
+      </c>
+      <c r="F125">
+        <v>5201</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B126">
+        <v>5609</v>
+      </c>
+      <c r="F126">
+        <v>5202</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B127">
+        <v>5631</v>
+      </c>
+      <c r="F127">
+        <v>5203</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B128">
+        <v>5640</v>
+      </c>
+      <c r="F128">
+        <v>5204</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B129">
+        <v>5641</v>
+      </c>
+      <c r="F129">
+        <v>5210</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B130">
+        <v>5652</v>
+      </c>
+      <c r="F130">
+        <v>5211</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B131">
+        <v>5680</v>
+      </c>
+      <c r="F131">
+        <v>5212</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B132">
+        <v>5690</v>
+      </c>
+      <c r="F132">
+        <v>5213</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B133">
+        <v>5700</v>
+      </c>
+      <c r="F133">
+        <v>5214</v>
+      </c>
+    </row>
+    <row r="134" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B134">
+        <v>5710</v>
+      </c>
+      <c r="F134">
+        <v>5220</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B135">
+        <v>5722</v>
+      </c>
+      <c r="F135">
+        <v>5221</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B136">
+        <v>5723</v>
+      </c>
+      <c r="F136">
+        <v>5222</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B137">
+        <v>5725</v>
+      </c>
+      <c r="F137">
+        <v>5223</v>
+      </c>
+    </row>
+    <row r="138" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B138">
+        <v>5731</v>
+      </c>
+      <c r="F138">
+        <v>5231</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F139">
+        <v>5232</v>
+      </c>
+    </row>
+    <row r="140" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F140">
+        <v>5233</v>
+      </c>
+    </row>
+    <row r="141" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F141">
+        <v>5234</v>
+      </c>
+    </row>
+    <row r="142" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F142">
+        <v>5235</v>
+      </c>
+    </row>
+    <row r="143" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F143">
+        <v>5238</v>
+      </c>
+    </row>
+    <row r="144" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F144">
+        <v>5241</v>
+      </c>
+    </row>
+    <row r="145" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F145">
+        <v>5242</v>
+      </c>
+    </row>
+    <row r="146" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F146">
+        <v>5243</v>
+      </c>
+    </row>
+    <row r="147" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F147">
+        <v>5244</v>
+      </c>
+    </row>
+    <row r="148" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F148">
+        <v>5245</v>
+      </c>
+    </row>
+    <row r="149" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F149">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="150" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F150">
+        <v>5251</v>
+      </c>
+    </row>
+    <row r="151" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F151">
+        <v>5252</v>
+      </c>
+    </row>
+    <row r="152" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F152">
+        <v>5253</v>
+      </c>
+    </row>
+    <row r="153" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F153">
+        <v>5254</v>
+      </c>
+    </row>
+    <row r="154" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F154">
+        <v>5255</v>
+      </c>
+    </row>
+    <row r="155" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F155">
+        <v>5256</v>
+      </c>
+    </row>
+    <row r="156" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F156">
+        <v>5259</v>
+      </c>
+    </row>
+    <row r="157" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F157">
+        <v>5260</v>
+      </c>
+    </row>
+    <row r="158" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F158">
+        <v>5263</v>
+      </c>
+    </row>
+    <row r="159" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F159">
+        <v>5264</v>
+      </c>
+    </row>
+    <row r="160" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F160">
+        <v>5266</v>
+      </c>
+    </row>
+    <row r="161" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F161">
+        <v>5267</v>
+      </c>
+    </row>
+    <row r="162" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F162">
+        <v>5268</v>
+      </c>
+    </row>
+    <row r="163" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F163">
+        <v>5269</v>
+      </c>
+    </row>
+    <row r="164" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F164">
+        <v>5270</v>
+      </c>
+    </row>
+    <row r="165" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F165">
+        <v>5271</v>
+      </c>
+    </row>
+    <row r="166" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F166">
+        <v>5273</v>
+      </c>
+    </row>
+    <row r="167" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F167">
+        <v>5275</v>
+      </c>
+    </row>
+    <row r="168" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F168">
+        <v>5276</v>
+      </c>
+    </row>
+    <row r="169" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F169">
+        <v>5277</v>
+      </c>
+    </row>
+    <row r="170" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F170">
+        <v>5280</v>
+      </c>
+    </row>
+    <row r="171" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F171">
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="172" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F172">
+        <v>5291</v>
+      </c>
+    </row>
+    <row r="173" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F173">
+        <v>5320</v>
+      </c>
+    </row>
+    <row r="174" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F174">
+        <v>5322</v>
+      </c>
+    </row>
+    <row r="175" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F175">
+        <v>5330</v>
+      </c>
+    </row>
+    <row r="176" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F176">
+        <v>5333</v>
+      </c>
+    </row>
+    <row r="177" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F177">
+        <v>5340</v>
+      </c>
+    </row>
+    <row r="178" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F178">
+        <v>5341</v>
+      </c>
+    </row>
+    <row r="179" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F179">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="180" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F180">
+        <v>5343</v>
+      </c>
+    </row>
+    <row r="181" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F181">
+        <v>5344</v>
+      </c>
+    </row>
+    <row r="182" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F182">
+        <v>5345</v>
+      </c>
+    </row>
+    <row r="183" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F183">
+        <v>5351</v>
+      </c>
+    </row>
+    <row r="184" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F184">
+        <v>5352</v>
+      </c>
+    </row>
+    <row r="185" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F185">
+        <v>5353</v>
+      </c>
+    </row>
+    <row r="186" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F186">
+        <v>5355</v>
+      </c>
+    </row>
+    <row r="187" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F187">
+        <v>5360</v>
+      </c>
+    </row>
+    <row r="188" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F188">
+        <v>5372</v>
+      </c>
+    </row>
+    <row r="189" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F189">
+        <v>5373</v>
+      </c>
+    </row>
+    <row r="190" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F190">
+        <v>5374</v>
+      </c>
+    </row>
+    <row r="191" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F191">
+        <v>5401</v>
+      </c>
+    </row>
+    <row r="192" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F192">
+        <v>5410</v>
+      </c>
+    </row>
+    <row r="193" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F193">
+        <v>5412</v>
+      </c>
+    </row>
+    <row r="194" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F194">
+        <v>5413</v>
+      </c>
+    </row>
+    <row r="195" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F195">
+        <v>5417</v>
+      </c>
+    </row>
+    <row r="196" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F196">
+        <v>5418</v>
+      </c>
+    </row>
+    <row r="197" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F197">
+        <v>5419</v>
+      </c>
+    </row>
+    <row r="198" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F198">
+        <v>5422</v>
+      </c>
+    </row>
+    <row r="199" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F199">
+        <v>5431</v>
+      </c>
+    </row>
+    <row r="200" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F200">
+        <v>5433</v>
+      </c>
+    </row>
+    <row r="201" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F201">
+        <v>5434</v>
+      </c>
+    </row>
+    <row r="202" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F202">
+        <v>5451</v>
+      </c>
+    </row>
+    <row r="203" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F203">
+        <v>5452</v>
+      </c>
+    </row>
+    <row r="204" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F204">
+        <v>5453</v>
+      </c>
+    </row>
+    <row r="205" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F205">
+        <v>5454</v>
+      </c>
+    </row>
+    <row r="206" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F206">
+        <v>5460</v>
+      </c>
+    </row>
+    <row r="207" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F207">
+        <v>5461</v>
+      </c>
+    </row>
+    <row r="208" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F208">
+        <v>5462</v>
+      </c>
+    </row>
+    <row r="209" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F209">
+        <v>5464</v>
+      </c>
+    </row>
+    <row r="210" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F210">
+        <v>5473</v>
+      </c>
+    </row>
+    <row r="211" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F211">
+        <v>5480</v>
+      </c>
+    </row>
+    <row r="212" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F212">
+        <v>5485</v>
+      </c>
+    </row>
+    <row r="213" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F213">
+        <v>5491</v>
+      </c>
+    </row>
+    <row r="214" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F214">
+        <v>5495</v>
+      </c>
+    </row>
+    <row r="215" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F215">
+        <v>5501</v>
+      </c>
+    </row>
+    <row r="216" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F216">
+        <v>5502</v>
+      </c>
+    </row>
+    <row r="217" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F217">
+        <v>5522</v>
+      </c>
+    </row>
+    <row r="218" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F218">
+        <v>5523</v>
+      </c>
+    </row>
+    <row r="219" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F219">
+        <v>5540</v>
+      </c>
+    </row>
+    <row r="220" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F220">
+        <v>5550</v>
+      </c>
+    </row>
+    <row r="221" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F221">
+        <v>5554</v>
+      </c>
+    </row>
+    <row r="222" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F222">
+        <v>5556</v>
+      </c>
+    </row>
+    <row r="223" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F223">
+        <v>5558</v>
+      </c>
+    </row>
+    <row r="224" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F224">
+        <v>5571</v>
+      </c>
+    </row>
+    <row r="225" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F225">
+        <v>5573</v>
+      </c>
+    </row>
+    <row r="226" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F226">
+        <v>5575</v>
+      </c>
+    </row>
+    <row r="227" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F227">
+        <v>5576</v>
+      </c>
+    </row>
+    <row r="228" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F228">
+        <v>5577</v>
+      </c>
+    </row>
+    <row r="229" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F229">
+        <v>5580</v>
+      </c>
+    </row>
+    <row r="230" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F230">
+        <v>5581</v>
+      </c>
+    </row>
+    <row r="231" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F231">
+        <v>5582</v>
+      </c>
+    </row>
+    <row r="232" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F232">
+        <v>5583</v>
+      </c>
+    </row>
+    <row r="233" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F233">
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="234" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F234">
+        <v>5602</v>
+      </c>
+    </row>
+    <row r="235" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F235">
+        <v>5603</v>
+      </c>
+    </row>
+    <row r="236" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F236">
+        <v>5604</v>
+      </c>
+    </row>
+    <row r="237" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F237">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="238" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F238">
+        <v>5606</v>
+      </c>
+    </row>
+    <row r="239" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F239">
+        <v>5607</v>
+      </c>
+    </row>
+    <row r="240" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F240">
+        <v>5608</v>
+      </c>
+    </row>
+    <row r="241" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F241">
+        <v>5609</v>
+      </c>
+    </row>
+    <row r="242" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F242">
+        <v>5630</v>
+      </c>
+    </row>
+    <row r="243" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F243">
+        <v>5631</v>
+      </c>
+    </row>
+    <row r="244" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F244">
+        <v>5640</v>
+      </c>
+    </row>
+    <row r="245" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F245">
+        <v>5641</v>
+      </c>
+    </row>
+    <row r="246" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F246">
+        <v>5652</v>
+      </c>
+    </row>
+    <row r="247" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F247">
+        <v>5680</v>
+      </c>
+    </row>
+    <row r="248" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F248">
+        <v>5690</v>
+      </c>
+    </row>
+    <row r="249" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F249">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="250" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F250">
+        <v>5710</v>
+      </c>
+    </row>
+    <row r="251" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F251">
+        <v>5723</v>
+      </c>
+    </row>
+    <row r="252" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F252">
+        <v>5725</v>
+      </c>
+    </row>
+    <row r="253" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F253">
+        <v>5731</v>
+      </c>
+    </row>
+    <row r="254" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F254" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="255" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F255" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
rent history graph plot
</commit_message>
<xml_diff>
--- a/rent_library.xlsx
+++ b/rent_library.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_R\Real_estate\real_estate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18661B9-7FE5-497A-A696-EB84B8C9FE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B769C725-ABB9-41CA-9ED2-E51FE95BF00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19010" yWindow="0" windowWidth="19380" windowHeight="20970" firstSheet="3" activeTab="6" xr2:uid="{07813744-485E-40CA-9C87-172D5E7C2A54}"/>
+    <workbookView xWindow="14580" yWindow="4500" windowWidth="28690" windowHeight="15340" firstSheet="1" activeTab="6" xr2:uid="{07813744-485E-40CA-9C87-172D5E7C2A54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="directory" sheetId="2" r:id="rId2"/>
-    <sheet name="directory_try" sheetId="5" r:id="rId3"/>
-    <sheet name="directory_2024" sheetId="7" r:id="rId4"/>
-    <sheet name="column_name_rename" sheetId="3" r:id="rId5"/>
-    <sheet name="rename_2011" sheetId="4" r:id="rId6"/>
-    <sheet name="rename_2024" sheetId="6" r:id="rId7"/>
-    <sheet name="metroX" sheetId="8" r:id="rId8"/>
+    <sheet name="directory_all" sheetId="9" r:id="rId3"/>
+    <sheet name="directory_try" sheetId="5" r:id="rId4"/>
+    <sheet name="directory_2024" sheetId="7" r:id="rId5"/>
+    <sheet name="column_name_rename" sheetId="3" r:id="rId6"/>
+    <sheet name="rename_2011" sheetId="4" r:id="rId7"/>
+    <sheet name="rename_2024" sheetId="6" r:id="rId8"/>
+    <sheet name="metroX" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="154">
   <si>
     <t>Quarter</t>
   </si>
@@ -420,9 +421,6 @@
     <t>4+ BR Houses</t>
   </si>
   <si>
-    <t>House unkown BR</t>
-  </si>
-  <si>
     <t>Total Houses</t>
   </si>
   <si>
@@ -504,10 +502,10 @@
     <t>Delete2</t>
   </si>
   <si>
-    <t>Total_Count</t>
-  </si>
-  <si>
-    <t>Total_Median</t>
+    <t>Rename</t>
+  </si>
+  <si>
+    <t>House unknown BR</t>
   </si>
 </sst>
 </file>
@@ -516,7 +514,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="170" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -565,7 +563,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1324,7 +1322,7 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1344,7 +1342,7 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1364,7 +1362,7 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1384,7 +1382,7 @@
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1404,7 +1402,7 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1424,7 +1422,7 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1444,7 +1442,7 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1464,7 +1462,7 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1484,7 +1482,7 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1504,7 +1502,7 @@
         <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1524,7 +1522,7 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1544,7 +1542,7 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1564,7 +1562,7 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1584,7 +1582,7 @@
         <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1604,7 +1602,7 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1624,7 +1622,7 @@
         <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1644,7 +1642,7 @@
         <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1664,7 +1662,7 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1684,7 +1682,7 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1704,7 +1702,7 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1724,7 +1722,7 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1744,7 +1742,7 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -1764,7 +1762,7 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1784,7 +1782,7 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1804,7 +1802,7 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -1824,7 +1822,7 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1844,7 +1842,7 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -1864,7 +1862,7 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1884,7 +1882,7 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1904,7 +1902,7 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1924,7 +1922,7 @@
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1944,7 +1942,7 @@
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1964,7 +1962,7 @@
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -1984,7 +1982,7 @@
         <v>19</v>
       </c>
       <c r="F35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -2004,7 +2002,7 @@
         <v>12</v>
       </c>
       <c r="F36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -2024,7 +2022,7 @@
         <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -2044,7 +2042,7 @@
         <v>12</v>
       </c>
       <c r="F38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -2064,7 +2062,7 @@
         <v>12</v>
       </c>
       <c r="F39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -2084,7 +2082,7 @@
         <v>12</v>
       </c>
       <c r="F40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -2352,11 +2350,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7862416-338A-4A69-9E9D-52FEB2010937}">
-  <dimension ref="A1:F58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC5859A-027F-49AC-AEC9-620CE611C0EA}">
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2382,7 +2380,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>64</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -2402,7 +2400,7 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -2422,7 +2420,7 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -2442,7 +2440,7 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -2462,7 +2460,7 @@
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2482,7 +2480,7 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -2502,7 +2500,7 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -2522,7 +2520,7 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -2542,7 +2540,7 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -2562,7 +2560,7 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -2582,7 +2580,7 @@
         <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2602,7 +2600,7 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2622,7 +2620,7 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -2642,7 +2640,7 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -2662,7 +2660,7 @@
         <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -2682,7 +2680,7 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -2702,7 +2700,7 @@
         <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -2722,7 +2720,7 @@
         <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -2742,7 +2740,7 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -2762,7 +2760,7 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -2782,7 +2780,7 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -2802,7 +2800,7 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -2822,7 +2820,7 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -2842,7 +2840,7 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -2862,7 +2860,7 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -2882,7 +2880,7 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -2902,7 +2900,7 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -2922,7 +2920,7 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -2942,7 +2940,7 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -2962,7 +2960,7 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -2982,7 +2980,7 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -3002,7 +3000,7 @@
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -3022,7 +3020,7 @@
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -3042,7 +3040,7 @@
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -3062,7 +3060,7 @@
         <v>19</v>
       </c>
       <c r="F35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -3082,7 +3080,7 @@
         <v>12</v>
       </c>
       <c r="F36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -3102,7 +3100,7 @@
         <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -3122,7 +3120,7 @@
         <v>12</v>
       </c>
       <c r="F38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -3142,7 +3140,7 @@
         <v>12</v>
       </c>
       <c r="F39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -3162,21 +3160,320 @@
         <v>12</v>
       </c>
       <c r="F40" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="3">
+        <v>44166</v>
+      </c>
+      <c r="D41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41">
+        <v>15</v>
+      </c>
+      <c r="F41" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="58" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="3">
+        <v>44256</v>
+      </c>
+      <c r="D42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42">
+        <v>15</v>
+      </c>
+      <c r="F42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="3">
+        <v>44348</v>
+      </c>
+      <c r="D43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43">
+        <v>15</v>
+      </c>
+      <c r="F43" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="3">
+        <v>44440</v>
+      </c>
+      <c r="D44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44">
+        <v>15</v>
+      </c>
+      <c r="F44" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="3">
+        <v>44531</v>
+      </c>
+      <c r="D45" t="s">
+        <v>63</v>
+      </c>
+      <c r="E45">
+        <v>15</v>
+      </c>
+      <c r="F45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="3">
+        <v>44621</v>
+      </c>
+      <c r="D46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="3">
+        <v>44713</v>
+      </c>
+      <c r="D47" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47">
+        <v>15</v>
+      </c>
+      <c r="F47" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="3">
+        <v>44805</v>
+      </c>
+      <c r="D48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48">
+        <v>15</v>
+      </c>
+      <c r="F48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="3">
+        <v>44896</v>
+      </c>
+      <c r="D49" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49">
+        <v>15</v>
+      </c>
+      <c r="F49" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="3">
+        <v>44986</v>
+      </c>
+      <c r="D50" t="s">
+        <v>63</v>
+      </c>
+      <c r="E50">
+        <v>16</v>
+      </c>
+      <c r="F50" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="3">
+        <v>45078</v>
+      </c>
+      <c r="D51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51">
+        <v>16</v>
+      </c>
+      <c r="F51" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="3">
+        <v>45170</v>
+      </c>
+      <c r="D52" t="s">
+        <v>63</v>
+      </c>
+      <c r="E52">
+        <v>16</v>
+      </c>
+      <c r="F52" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="3">
+        <v>45261</v>
+      </c>
+      <c r="D53" t="s">
+        <v>63</v>
+      </c>
+      <c r="E53">
+        <v>15</v>
+      </c>
+      <c r="F53" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="3">
+        <v>45352</v>
+      </c>
+      <c r="D54" t="s">
+        <v>63</v>
+      </c>
+      <c r="E54">
+        <v>15</v>
+      </c>
+      <c r="F54" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>57</v>
+      </c>
+      <c r="C55" s="3">
+        <v>45444</v>
+      </c>
+      <c r="D55" t="s">
+        <v>63</v>
+      </c>
+      <c r="E55">
+        <v>15</v>
+      </c>
+      <c r="F55" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C773356D-0F65-45D6-94FD-903551291D21}">
-  <dimension ref="A1:F40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7862416-338A-4A69-9E9D-52FEB2010937}">
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3207,382 +3504,1202 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3">
-        <v>44166</v>
+        <v>40513</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3">
-        <v>44256</v>
+        <v>40603</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3">
-        <v>44348</v>
+        <v>40695</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3">
-        <v>44440</v>
+        <v>40787</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3">
-        <v>44531</v>
+        <v>40878</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3">
-        <v>44621</v>
+        <v>40969</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3">
-        <v>44713</v>
+        <v>41061</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3">
-        <v>44805</v>
+        <v>41153</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3">
-        <v>44896</v>
+        <v>41244</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3">
-        <v>44986</v>
+        <v>41334</v>
       </c>
       <c r="D11" t="s">
         <v>63</v>
       </c>
       <c r="E11">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3">
-        <v>45078</v>
+        <v>41426</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E12">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3">
-        <v>45170</v>
+        <v>41518</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E13">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C14" s="3">
-        <v>45261</v>
+        <v>41609</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E14">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3">
-        <v>45352</v>
+        <v>41699</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3">
-        <v>45444</v>
+        <v>41791</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="3">
+        <v>41883</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3">
+        <v>41974</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3">
+        <v>42064</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3">
+        <v>42156</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="3">
+        <v>42248</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="3">
+        <v>42339</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="3">
+        <v>42430</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="3">
+        <v>42522</v>
+      </c>
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24">
+        <v>19</v>
+      </c>
+      <c r="F24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="3">
+        <v>42614</v>
+      </c>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="3">
+        <v>42705</v>
+      </c>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26">
+        <v>19</v>
+      </c>
+      <c r="F26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="3">
+        <v>42795</v>
+      </c>
+      <c r="D27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="3">
+        <v>42887</v>
+      </c>
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28">
+        <v>19</v>
+      </c>
+      <c r="F28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="3">
+        <v>42979</v>
+      </c>
+      <c r="D29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29">
+        <v>19</v>
+      </c>
+      <c r="F29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="3">
+        <v>43070</v>
+      </c>
+      <c r="D30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30">
+        <v>19</v>
+      </c>
+      <c r="F30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="3">
+        <v>43160</v>
+      </c>
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31">
+        <v>19</v>
+      </c>
+      <c r="F31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="3">
+        <v>43344</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="3">
+        <v>43435</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="3">
+        <v>43525</v>
+      </c>
+      <c r="D34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34">
+        <v>19</v>
+      </c>
+      <c r="F34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="3">
+        <v>43617</v>
+      </c>
+      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35">
+        <v>19</v>
+      </c>
+      <c r="F35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>15</v>
       </c>
-      <c r="F16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C40" s="3"/>
-    </row>
+      <c r="C36" s="3">
+        <v>43709</v>
+      </c>
+      <c r="D36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="3">
+        <v>43800</v>
+      </c>
+      <c r="D37" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37">
+        <v>12</v>
+      </c>
+      <c r="F37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="3">
+        <v>43891</v>
+      </c>
+      <c r="D38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="3">
+        <v>43983</v>
+      </c>
+      <c r="D39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="3">
+        <v>44075</v>
+      </c>
+      <c r="D40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40">
+        <v>12</v>
+      </c>
+      <c r="F40" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C773356D-0F65-45D6-94FD-903551291D21}">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="54.90625" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44166</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3">
+        <v>44256</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44348</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44440</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44531</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="3">
+        <v>44621</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44713</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44805</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3">
+        <v>44896</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3">
+        <v>44986</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45078</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45170</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45261</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45352</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45444</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C40" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B2B4F8-84A7-42A5-AD2F-D10CF868A00A}">
   <dimension ref="B1:B7"/>
   <sheetViews>
@@ -3636,12 +4753,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65798D6-DDCA-4973-BAFA-2D28352840F3}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3723,7 +4840,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
         <v>73</v>
@@ -3835,7 +4952,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>153</v>
       </c>
       <c r="B24" t="s">
         <v>87</v>
@@ -3851,7 +4968,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
         <v>89</v>
@@ -3910,12 +5027,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9392492D-C307-4343-BED9-8FAD1A381722}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3950,7 +5067,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
         <v>67</v>
@@ -3958,7 +5075,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
         <v>70</v>
@@ -3974,7 +5091,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
         <v>69</v>
@@ -3990,7 +5107,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
         <v>72</v>
@@ -4006,7 +5123,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
@@ -4022,7 +5139,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B13" t="s">
         <v>76</v>
@@ -4038,7 +5155,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B15" t="s">
         <v>78</v>
@@ -4054,7 +5171,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B17" t="s">
         <v>80</v>
@@ -4070,7 +5187,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B19" t="s">
         <v>82</v>
@@ -4086,7 +5203,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
         <v>84</v>
@@ -4102,7 +5219,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B23" t="s">
         <v>86</v>
@@ -4118,7 +5235,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B25" t="s">
         <v>88</v>
@@ -4134,7 +5251,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B27" t="s">
         <v>90</v>
@@ -4150,7 +5267,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29" t="s">
         <v>96</v>
@@ -4161,15 +5278,15 @@
         <v>113</v>
       </c>
       <c r="B30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -4177,15 +5294,15 @@
         <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>153</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -4201,7 +5318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9415D53-1FA2-499A-BD09-F544ECCD8C23}">
   <dimension ref="A1:F255"/>
   <sheetViews>
@@ -4216,7 +5333,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -5508,7 +6625,7 @@
         <v>5600</v>
       </c>
       <c r="F119" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
@@ -5516,7 +6633,7 @@
         <v>5602</v>
       </c>
       <c r="F120" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
@@ -6240,12 +7357,12 @@
     </row>
     <row r="254" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F254" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="255" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F255" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>